<commit_message>
Fixed formula spreading. Added some crash checks.
</commit_message>
<xml_diff>
--- a/examples/formula-output.xlsx
+++ b/examples/formula-output.xlsx
@@ -7,7 +7,8 @@
   <sheets>
     <sheet name="NoRef" sheetId="1" r:id="rId4"/>
     <sheet name="Ref" sheetId="2" r:id="rId5"/>
-    <sheet name="Empty" sheetId="3" r:id="rId6"/>
+    <sheet name="Split" sheetId="3" r:id="rId6"/>
+    <sheet name="Empty" sheetId="4" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -46,6 +47,15 @@
   </si>
   <si>
     <t>{{ B2 | all | =B2 * $A$6 }}</t>
+  </si>
+  <si>
+    <t>{{ A2 | 1 * data | }}</t>
+  </si>
+  <si>
+    <t>{{ B2 || =SUM(B2:B2) * $A$6 }}</t>
+  </si>
+  <si>
+    <t>:with external</t>
   </si>
   <si>
     <t xml:space="preserve">An exemplary title</t>
@@ -172,6 +182,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -221,6 +261,18 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -241,6 +293,7 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1319,7 +1372,7 @@
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -1329,7 +1382,7 @@
     </row>
     <row r="2" ht="20.05" customHeight="1">
       <c r="A2" t="s" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" s="6">
         <v>11</v>
@@ -1349,7 +1402,7 @@
     </row>
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6">
         <v>21</v>
@@ -1369,7 +1422,7 @@
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="5">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B4" s="6">
         <v>31</v>
@@ -1550,7 +1603,7 @@
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -1560,7 +1613,7 @@
     </row>
     <row r="2" ht="20.05" customHeight="1">
       <c r="A2" t="s" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" s="6">
         <v>11</v>
@@ -1580,7 +1633,7 @@
     </row>
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6">
         <v>21</v>
@@ -1600,7 +1653,7 @@
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="5">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B4" s="6">
         <v>31</v>
@@ -1827,6 +1880,235 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="6" width="16.3516" style="13" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20.25" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" ht="20.05" customHeight="1">
+      <c r="A2" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6">
+        <v>13</v>
+      </c>
+      <c r="E2" s="6">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6">
+        <v>22</v>
+      </c>
+      <c r="D3" s="6">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" t="s" s="5">
+        <v>17</v>
+      </c>
+      <c r="B4" s="6">
+        <v>31</v>
+      </c>
+      <c r="C4" s="6">
+        <v>32</v>
+      </c>
+      <c r="D4" s="6">
+        <v>33</v>
+      </c>
+      <c r="E4" s="6">
+        <v>34</v>
+      </c>
+      <c r="F4" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="11">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" t="s" s="12">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6">
+        <f>SUM(B2:F2)</f>
+      </c>
+      <c r="C7" s="14">
+        <f>SUM(B2:F2) * $A$6</f>
+      </c>
+      <c r="D7" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="16"/>
+      <c r="B8" s="6">
+        <f>SUM(B3:F3)</f>
+      </c>
+      <c r="C8" s="7">
+        <f>SUM(B3:F3) * $A$6</f>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="7">
+        <f>SUM(B4:F4)</f>
+      </c>
+      <c r="C9" s="7">
+        <f>SUM(B4:F4) * $A$6</f>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="8"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1835,8 +2117,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="13" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="17" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.7" customHeight="1">

</xml_diff>